<commit_message>
removed normalisation on loadcell 7, new comparison start of not normalised, v5 is still leading
</commit_message>
<xml_diff>
--- a/Data/Run_10-6.xlsx
+++ b/Data/Run_10-6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BEP-Autonomous Irrigation\BEP-Autonomous-Irrigation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\BEP-Autonomous-Irrigation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82FB63-8832-4B94-8A4A-1334F6C36F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD3EC08-988D-40F6-B874-96B4B3C8BEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="3255" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1423,16 +1423,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="K338" sqref="K338"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>23.48</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>22.65</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>22.37</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>22.67</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>22.71</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>22.83</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>22.87</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>22.94</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>22.94</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>22.97</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>23.03</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>23.12</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>23.34</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>23.42</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>23.27</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>23.27</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>23.27</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>23.15</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>23.09</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>23.11</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>23.19</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>23.19</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>23.13</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>23.16</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>23.22</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>23.09</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>23.11</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>23.12</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>23.18</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>23.39</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>23.39</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>23.44</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>23.34</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>23.19</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>22.83</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>22.71</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>22.58</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>22.69</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>22.77</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>22.66</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>22.57</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>105</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>22.54</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>23.41</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>23.52</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>23.44</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>23.54</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>23.43</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>23.65</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>23.74</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>23.72</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>23.63</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>23.72</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>23.74</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>23.62</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>23.79</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>23.87</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>23.92</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>23.96</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>125</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>23.76</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>23.93</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>23.84</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>23.82</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>23.92</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>23.89</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>23.81</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>23.67</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>23.66</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>23.34</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>23.65</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>23.77</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>23.54</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>23.55</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>23.29</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>23.65</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>23.63</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -8936,7 +8936,7 @@
         <v>23.49</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -8992,7 +8992,7 @@
         <v>23.85</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>23.58</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -9160,7 +9160,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>23.72</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>23.63</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>23.74</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>23.68</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -9496,7 +9496,7 @@
         <v>23.93</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -9552,7 +9552,7 @@
         <v>24.04</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>24.16</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>23.53</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>23.46</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -9776,7 +9776,7 @@
         <v>23.11</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>23.26</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -9888,7 +9888,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>23.08</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>23.05</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>168</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>169</v>
       </c>
@@ -10112,7 +10112,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>23.39</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>23.36</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>23.22</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -10392,7 +10392,7 @@
         <v>23.15</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>23.33</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -10560,7 +10560,7 @@
         <v>22.94</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>23.13</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -10728,7 +10728,7 @@
         <v>23.16</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>181</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>23.21</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>182</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>23.09</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>183</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>23.02</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>184</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>23.06</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>185</v>
       </c>
@@ -11008,7 +11008,7 @@
         <v>23.16</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -11064,7 +11064,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>187</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -11176,7 +11176,7 @@
         <v>22.99</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>189</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -11288,7 +11288,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -11344,7 +11344,7 @@
         <v>22.95</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>23.01</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -11456,7 +11456,7 @@
         <v>22.98</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -11512,7 +11512,7 @@
         <v>22.94</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -11568,7 +11568,7 @@
         <v>22.97</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>196</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>22.87</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>197</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>198</v>
       </c>
@@ -11736,7 +11736,7 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>199</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>22.79</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>200</v>
       </c>
@@ -11848,7 +11848,7 @@
         <v>22.79</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>201</v>
       </c>
@@ -11904,7 +11904,7 @@
         <v>22.77</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>202</v>
       </c>
@@ -11960,7 +11960,7 @@
         <v>22.76</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>203</v>
       </c>
@@ -12016,7 +12016,7 @@
         <v>22.76</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>204</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>205</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>22.72</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>206</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>22.73</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>207</v>
       </c>
@@ -12240,7 +12240,7 @@
         <v>22.65</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>208</v>
       </c>
@@ -12296,7 +12296,7 @@
         <v>22.62</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>209</v>
       </c>
@@ -12352,7 +12352,7 @@
         <v>22.59</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>210</v>
       </c>
@@ -12408,7 +12408,7 @@
         <v>22.59</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>211</v>
       </c>
@@ -12464,7 +12464,7 @@
         <v>22.59</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>212</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>213</v>
       </c>
@@ -12576,7 +12576,7 @@
         <v>22.49</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>214</v>
       </c>
@@ -12632,7 +12632,7 @@
         <v>22.47</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>215</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>216</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>22.46</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>217</v>
       </c>
@@ -12800,7 +12800,7 @@
         <v>22.46</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>218</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>22.44</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>219</v>
       </c>
@@ -12912,7 +12912,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>220</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>22.38</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>221</v>
       </c>
@@ -13024,7 +13024,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>222</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>22.41</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>223</v>
       </c>
@@ -13136,7 +13136,7 @@
         <v>22.35</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>224</v>
       </c>
@@ -13192,7 +13192,7 @@
         <v>22.33</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>225</v>
       </c>
@@ -13248,7 +13248,7 @@
         <v>22.43</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>226</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>22.32</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>227</v>
       </c>
@@ -13360,7 +13360,7 @@
         <v>22.37</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>228</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>22.32</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>229</v>
       </c>
@@ -13472,7 +13472,7 @@
         <v>22.34</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>230</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>22.27</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>231</v>
       </c>
@@ -13584,7 +13584,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>232</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>22.19</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>233</v>
       </c>
@@ -13696,7 +13696,7 @@
         <v>22.15</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>234</v>
       </c>
@@ -13752,7 +13752,7 @@
         <v>22.06</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>235</v>
       </c>
@@ -13808,7 +13808,7 @@
         <v>22.13</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>236</v>
       </c>
@@ -13864,7 +13864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>237</v>
       </c>
@@ -13920,7 +13920,7 @@
         <v>22.15</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>238</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>22.03</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>239</v>
       </c>
@@ -14032,7 +14032,7 @@
         <v>22.03</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>240</v>
       </c>
@@ -14088,7 +14088,7 @@
         <v>22.07</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>241</v>
       </c>
@@ -14144,7 +14144,7 @@
         <v>22.04</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>242</v>
       </c>
@@ -14200,7 +14200,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>243</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>21.96</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>244</v>
       </c>
@@ -14312,7 +14312,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>245</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>21.92</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>246</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>21.91</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>247</v>
       </c>
@@ -14480,7 +14480,7 @@
         <v>21.86</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>248</v>
       </c>
@@ -14536,7 +14536,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>249</v>
       </c>
@@ -14592,7 +14592,7 @@
         <v>21.82</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>250</v>
       </c>
@@ -14648,7 +14648,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>251</v>
       </c>
@@ -14704,7 +14704,7 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>252</v>
       </c>
@@ -14760,7 +14760,7 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>253</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>254</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>21.82</v>
       </c>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>255</v>
       </c>
@@ -14928,7 +14928,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>256</v>
       </c>
@@ -14984,7 +14984,7 @@
         <v>21.66</v>
       </c>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>257</v>
       </c>
@@ -15040,7 +15040,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>258</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>259</v>
       </c>
@@ -15152,7 +15152,7 @@
         <v>21.63</v>
       </c>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>260</v>
       </c>
@@ -15208,7 +15208,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>261</v>
       </c>
@@ -15264,7 +15264,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>262</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>21.66</v>
       </c>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>263</v>
       </c>
@@ -15376,7 +15376,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>264</v>
       </c>
@@ -15432,7 +15432,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>265</v>
       </c>
@@ -15488,7 +15488,7 @@
         <v>21.58</v>
       </c>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>266</v>
       </c>
@@ -15544,7 +15544,7 @@
         <v>21.59</v>
       </c>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>267</v>
       </c>
@@ -15600,7 +15600,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>268</v>
       </c>
@@ -15656,7 +15656,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>269</v>
       </c>
@@ -15712,7 +15712,7 @@
         <v>21.55</v>
       </c>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>270</v>
       </c>
@@ -15768,7 +15768,7 @@
         <v>21.48</v>
       </c>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>271</v>
       </c>
@@ -15824,7 +15824,7 @@
         <v>21.56</v>
       </c>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>272</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>21.49</v>
       </c>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>273</v>
       </c>
@@ -15936,7 +15936,7 @@
         <v>21.46</v>
       </c>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>274</v>
       </c>
@@ -15992,7 +15992,7 @@
         <v>21.51</v>
       </c>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>275</v>
       </c>
@@ -16048,7 +16048,7 @@
         <v>21.44</v>
       </c>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>276</v>
       </c>
@@ -16104,7 +16104,7 @@
         <v>21.48</v>
       </c>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>277</v>
       </c>
@@ -16160,7 +16160,7 @@
         <v>21.41</v>
       </c>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>278</v>
       </c>
@@ -16216,7 +16216,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>279</v>
       </c>
@@ -16272,7 +16272,7 @@
         <v>21.45</v>
       </c>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>280</v>
       </c>
@@ -16328,7 +16328,7 @@
         <v>21.38</v>
       </c>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>281</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>282</v>
       </c>
@@ -16440,7 +16440,7 @@
         <v>21.33</v>
       </c>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>283</v>
       </c>
@@ -16496,7 +16496,7 @@
         <v>21.31</v>
       </c>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>284</v>
       </c>
@@ -16552,7 +16552,7 @@
         <v>21.37</v>
       </c>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>285</v>
       </c>
@@ -16608,7 +16608,7 @@
         <v>21.29</v>
       </c>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>286</v>
       </c>
@@ -16664,7 +16664,7 @@
         <v>21.26</v>
       </c>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>287</v>
       </c>
@@ -16720,7 +16720,7 @@
         <v>21.27</v>
       </c>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>288</v>
       </c>
@@ -16776,7 +16776,7 @@
         <v>21.27</v>
       </c>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>289</v>
       </c>
@@ -16832,7 +16832,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>290</v>
       </c>
@@ -16888,7 +16888,7 @@
         <v>21.22</v>
       </c>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>291</v>
       </c>
@@ -16944,7 +16944,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>292</v>
       </c>
@@ -17000,7 +17000,7 @@
         <v>21.22</v>
       </c>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>293</v>
       </c>
@@ -17056,7 +17056,7 @@
         <v>21.21</v>
       </c>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>294</v>
       </c>
@@ -17112,7 +17112,7 @@
         <v>21.22</v>
       </c>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>295</v>
       </c>
@@ -17168,7 +17168,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>296</v>
       </c>
@@ -17224,7 +17224,7 @@
         <v>21.15</v>
       </c>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>297</v>
       </c>
@@ -17280,7 +17280,7 @@
         <v>21.06</v>
       </c>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>298</v>
       </c>
@@ -17336,7 +17336,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>299</v>
       </c>
@@ -17392,7 +17392,7 @@
         <v>21.09</v>
       </c>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>300</v>
       </c>
@@ -17448,7 +17448,7 @@
         <v>21.07</v>
       </c>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>301</v>
       </c>
@@ -17504,7 +17504,7 @@
         <v>21.13</v>
       </c>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>302</v>
       </c>
@@ -17560,7 +17560,7 @@
         <v>21.13</v>
       </c>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>303</v>
       </c>
@@ -17616,7 +17616,7 @@
         <v>21.18</v>
       </c>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>304</v>
       </c>
@@ -17672,7 +17672,7 @@
         <v>21.17</v>
       </c>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>305</v>
       </c>
@@ -17728,7 +17728,7 @@
         <v>21.28</v>
       </c>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>306</v>
       </c>
@@ -17784,7 +17784,7 @@
         <v>21.33</v>
       </c>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>307</v>
       </c>
@@ -17840,7 +17840,7 @@
         <v>21.41</v>
       </c>
     </row>
-    <row r="294" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>308</v>
       </c>
@@ -17896,7 +17896,7 @@
         <v>21.43</v>
       </c>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>309</v>
       </c>
@@ -17952,7 +17952,7 @@
         <v>21.52</v>
       </c>
     </row>
-    <row r="296" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>310</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>21.52</v>
       </c>
     </row>
-    <row r="297" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>311</v>
       </c>
@@ -18064,7 +18064,7 @@
         <v>21.56</v>
       </c>
     </row>
-    <row r="298" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>312</v>
       </c>
@@ -18120,7 +18120,7 @@
         <v>21.43</v>
       </c>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>313</v>
       </c>
@@ -18176,7 +18176,7 @@
         <v>21.52</v>
       </c>
     </row>
-    <row r="300" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>314</v>
       </c>
@@ -18232,7 +18232,7 @@
         <v>21.52</v>
       </c>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>315</v>
       </c>
@@ -18288,7 +18288,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>316</v>
       </c>
@@ -18344,7 +18344,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>317</v>
       </c>
@@ -18400,7 +18400,7 @@
         <v>21.47</v>
       </c>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>318</v>
       </c>
@@ -18456,7 +18456,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>319</v>
       </c>
@@ -18512,7 +18512,7 @@
         <v>21.45</v>
       </c>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>320</v>
       </c>
@@ -18568,7 +18568,7 @@
         <v>21.56</v>
       </c>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>321</v>
       </c>
@@ -18624,7 +18624,7 @@
         <v>21.52</v>
       </c>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>322</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>21.78</v>
       </c>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>323</v>
       </c>
@@ -18736,7 +18736,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="310" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>324</v>
       </c>
@@ -18792,7 +18792,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>325</v>
       </c>
@@ -18848,7 +18848,7 @@
         <v>22.27</v>
       </c>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>326</v>
       </c>
@@ -18904,7 +18904,7 @@
         <v>22.31</v>
       </c>
     </row>
-    <row r="313" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>327</v>
       </c>
@@ -18960,7 +18960,7 @@
         <v>22.33</v>
       </c>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>328</v>
       </c>
@@ -19016,7 +19016,7 @@
         <v>22.39</v>
       </c>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>329</v>
       </c>
@@ -19072,7 +19072,7 @@
         <v>22.48</v>
       </c>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>330</v>
       </c>
@@ -19128,7 +19128,7 @@
         <v>22.62</v>
       </c>
     </row>
-    <row r="317" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>331</v>
       </c>
@@ -19184,7 +19184,7 @@
         <v>22.68</v>
       </c>
     </row>
-    <row r="318" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>332</v>
       </c>
@@ -19240,7 +19240,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="319" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>333</v>
       </c>
@@ -19296,7 +19296,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="320" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>334</v>
       </c>
@@ -19352,7 +19352,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>335</v>
       </c>
@@ -19408,7 +19408,7 @@
         <v>22.79</v>
       </c>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>336</v>
       </c>
@@ -19464,7 +19464,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>337</v>
       </c>
@@ -19520,7 +19520,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="324" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>338</v>
       </c>
@@ -19576,7 +19576,7 @@
         <v>23.08</v>
       </c>
     </row>
-    <row r="325" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>339</v>
       </c>
@@ -19632,7 +19632,7 @@
         <v>23.18</v>
       </c>
     </row>
-    <row r="326" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>340</v>
       </c>
@@ -19688,7 +19688,7 @@
         <v>23.09</v>
       </c>
     </row>
-    <row r="327" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>341</v>
       </c>
@@ -19744,7 +19744,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="328" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>342</v>
       </c>
@@ -19800,7 +19800,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="329" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>343</v>
       </c>
@@ -19856,7 +19856,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="330" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>344</v>
       </c>
@@ -19912,7 +19912,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="331" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>345</v>
       </c>
@@ -19968,7 +19968,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="332" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>346</v>
       </c>
@@ -20024,7 +20024,7 @@
         <v>23.53</v>
       </c>
     </row>
-    <row r="333" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>347</v>
       </c>
@@ -20080,7 +20080,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="334" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>348</v>
       </c>
@@ -20136,7 +20136,7 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="335" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>349</v>
       </c>
@@ -20192,7 +20192,7 @@
         <v>23.52</v>
       </c>
     </row>
-    <row r="336" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>350</v>
       </c>
@@ -20248,7 +20248,7 @@
         <v>23.49</v>
       </c>
     </row>
-    <row r="337" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>351</v>
       </c>
@@ -20304,7 +20304,7 @@
         <v>23.52</v>
       </c>
     </row>
-    <row r="338" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>352</v>
       </c>
@@ -20360,7 +20360,7 @@
         <v>23.67</v>
       </c>
     </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>353</v>
       </c>
@@ -20422,6 +20422,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004E415049872CFD40BDAE2144929C1E5B" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="f9a140c8d32ab5d104c615cc6b97ee67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f38184ff-deff-47ac-868c-dfb8bb8b29b2" xmlns:ns3="343cd848-1fd6-48cb-97d5-5d23ebd699f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="691be60b6cfbba6245aead64dbab5403" ns2:_="" ns3:_="">
     <xsd:import namespace="f38184ff-deff-47ac-868c-dfb8bb8b29b2"/>
@@ -20628,15 +20637,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -20649,6 +20649,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DB81809-0AEE-4818-80BE-BE8B86B7A34A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F64E9F0-40A7-4F55-9FBB-04FE27724F9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20667,14 +20675,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DB81809-0AEE-4818-80BE-BE8B86B7A34A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D628B2-E76B-4328-B138-428B38AFC464}">
   <ds:schemaRefs>

</xml_diff>